<commit_message>
add chart and readme
</commit_message>
<xml_diff>
--- a/PVT.xlsx
+++ b/PVT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\pollster.ge\Geo Parl 2020\Analysis\PVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732C3B5A-3C46-426B-8ADF-806B5144788B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6207102C-6ED0-4E23-B26A-E70717F48D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B9C24D5-4B9D-4AB9-A329-993DCFBFA6B6}"/>
   </bookViews>
@@ -288,12 +288,6 @@
     <t>MoE</t>
   </si>
   <si>
-    <t>2018 Presidential 1</t>
-  </si>
-  <si>
-    <t>2018 Presidential 2</t>
-  </si>
-  <si>
     <t>2013 Presidential</t>
   </si>
   <si>
@@ -355,6 +349,12 @@
   </si>
   <si>
     <t>New Rights</t>
+  </si>
+  <si>
+    <t>2018 Presidential 1st round</t>
+  </si>
+  <si>
+    <t>2018 Presidential 2nd round (runoff)</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -402,7 +402,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ჩვეულებრივი" xfId="0" builtinId="0"/>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE21F1AA-B01C-4C72-8421-86648BE89CF2}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,10 +758,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>26.6</v>
@@ -775,10 +775,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
       </c>
       <c r="C3">
         <v>18.920000000000002</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -809,10 +809,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>10.15</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7">
         <v>7.99</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -869,11 +869,11 @@
         <v>67.78</v>
       </c>
       <c r="D8">
-        <f>C8-F8</f>
+        <f t="shared" ref="D8:D14" si="0">C8-F8</f>
         <v>67.73</v>
       </c>
       <c r="E8">
-        <f>C8+F8</f>
+        <f t="shared" ref="E8:E14" si="1">C8+F8</f>
         <v>67.83</v>
       </c>
       <c r="F8">
@@ -888,7 +888,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -897,11 +897,11 @@
         <v>7.75</v>
       </c>
       <c r="D9">
-        <f>C9-F9</f>
+        <f t="shared" si="0"/>
         <v>7.7</v>
       </c>
       <c r="E9">
-        <f>C9+F9</f>
+        <f t="shared" si="1"/>
         <v>7.8</v>
       </c>
       <c r="F9">
@@ -916,7 +916,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -925,11 +925,11 @@
         <v>6.6</v>
       </c>
       <c r="D10">
-        <f>C10-F10</f>
+        <f t="shared" si="0"/>
         <v>6.55</v>
       </c>
       <c r="E10">
-        <f>C10+F10</f>
+        <f t="shared" si="1"/>
         <v>6.6499999999999995</v>
       </c>
       <c r="F10">
@@ -944,7 +944,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -953,11 +953,11 @@
         <v>6.14</v>
       </c>
       <c r="D11">
-        <f>C11-F11</f>
+        <f t="shared" si="0"/>
         <v>6.09</v>
       </c>
       <c r="E11">
-        <f>C11+F11</f>
+        <f t="shared" si="1"/>
         <v>6.1899999999999995</v>
       </c>
       <c r="F11">
@@ -972,7 +972,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -981,11 +981,11 @@
         <v>4.72</v>
       </c>
       <c r="D12">
-        <f>C12-F12</f>
+        <f t="shared" si="0"/>
         <v>4.67</v>
       </c>
       <c r="E12">
-        <f>C12+F12</f>
+        <f t="shared" si="1"/>
         <v>4.7699999999999996</v>
       </c>
       <c r="F12">
@@ -1000,7 +1000,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1009,11 +1009,11 @@
         <v>2.38</v>
       </c>
       <c r="D13">
-        <f>C13-F13</f>
+        <f t="shared" si="0"/>
         <v>2.33</v>
       </c>
       <c r="E13">
-        <f>C13+F13</f>
+        <f t="shared" si="1"/>
         <v>2.4299999999999997</v>
       </c>
       <c r="F13">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1037,11 +1037,11 @@
         <v>2.19</v>
       </c>
       <c r="D14">
-        <f>C14-F14</f>
+        <f t="shared" si="0"/>
         <v>2.14</v>
       </c>
       <c r="E14">
-        <f>C14+F14</f>
+        <f t="shared" si="1"/>
         <v>2.2399999999999998</v>
       </c>
       <c r="F14">
@@ -1056,7 +1056,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -1073,10 +1073,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>1.93</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
         <v>96</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
       </c>
       <c r="C18">
         <v>0.22</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19">
         <v>0.16</v>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20">
         <v>7.0000000000000007E-2</v>
@@ -1158,10 +1158,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21">
         <v>0.32</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1192,10 +1192,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23">
         <v>12.14</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
         <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
       </c>
       <c r="C25">
         <v>6.22</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <v>2.82</v>
@@ -1260,10 +1260,10 @@
     </row>
     <row r="27" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27">
         <v>0.02</v>
@@ -1277,10 +1277,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C28">
         <v>0.99</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
         <v>27</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
         <v>28</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
         <v>30</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
@@ -1507,11 +1507,11 @@
         <v>50.8</v>
       </c>
       <c r="D41">
-        <f>C41-F41</f>
+        <f t="shared" ref="D41:D52" si="2">C41-F41</f>
         <v>50.779999999999994</v>
       </c>
       <c r="E41">
-        <f>C41+F41</f>
+        <f t="shared" ref="E41:E52" si="3">C41+F41</f>
         <v>50.82</v>
       </c>
       <c r="F41">
@@ -1526,7 +1526,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
@@ -1535,11 +1535,11 @@
         <v>27.2</v>
       </c>
       <c r="D42">
-        <f>C42-F42</f>
+        <f t="shared" si="2"/>
         <v>27.18</v>
       </c>
       <c r="E42">
-        <f>C42+F42</f>
+        <f t="shared" si="3"/>
         <v>27.22</v>
       </c>
       <c r="F42">
@@ -1554,7 +1554,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
         <v>21</v>
@@ -1563,11 +1563,11 @@
         <v>7.3</v>
       </c>
       <c r="D43">
-        <f>C43-F43</f>
+        <f t="shared" si="2"/>
         <v>7.28</v>
       </c>
       <c r="E43">
-        <f>C43+F43</f>
+        <f t="shared" si="3"/>
         <v>7.3199999999999994</v>
       </c>
       <c r="F43">
@@ -1582,7 +1582,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -1591,11 +1591,11 @@
         <v>7</v>
       </c>
       <c r="D44">
-        <f>C44-F44</f>
+        <f t="shared" si="2"/>
         <v>6.98</v>
       </c>
       <c r="E44">
-        <f>C44+F44</f>
+        <f t="shared" si="3"/>
         <v>7.02</v>
       </c>
       <c r="F44">
@@ -1610,7 +1610,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -1619,11 +1619,11 @@
         <v>4.3</v>
       </c>
       <c r="D45">
-        <f>C45-F45</f>
+        <f t="shared" si="2"/>
         <v>4.28</v>
       </c>
       <c r="E45">
-        <f>C45+F45</f>
+        <f t="shared" si="3"/>
         <v>4.3199999999999994</v>
       </c>
       <c r="F45">
@@ -1638,7 +1638,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -1647,11 +1647,11 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <f>C46-F46</f>
+        <f t="shared" si="2"/>
         <v>0.98</v>
       </c>
       <c r="E46">
-        <f>C46+F46</f>
+        <f t="shared" si="3"/>
         <v>1.02</v>
       </c>
       <c r="F46">
@@ -1666,7 +1666,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1675,11 +1675,11 @@
         <v>0.2</v>
       </c>
       <c r="D47">
-        <f>C47-F47</f>
+        <f t="shared" si="2"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="E47">
-        <f>C47+F47</f>
+        <f t="shared" si="3"/>
         <v>0.22</v>
       </c>
       <c r="F47">
@@ -1694,7 +1694,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -1703,11 +1703,11 @@
         <v>40.700000000000003</v>
       </c>
       <c r="D48">
-        <f>C48-F48</f>
+        <f t="shared" si="2"/>
         <v>40.690000000000005</v>
       </c>
       <c r="E48">
-        <f>C48+F48</f>
+        <f t="shared" si="3"/>
         <v>40.71</v>
       </c>
       <c r="F48">
@@ -1722,7 +1722,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -1731,11 +1731,11 @@
         <v>54.6</v>
       </c>
       <c r="D49">
-        <f>C49-F49</f>
+        <f t="shared" si="2"/>
         <v>54.59</v>
       </c>
       <c r="E49">
-        <f>C49+F49</f>
+        <f t="shared" si="3"/>
         <v>54.61</v>
       </c>
       <c r="F49">
@@ -1750,7 +1750,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -1759,11 +1759,11 @@
         <v>2</v>
       </c>
       <c r="D50">
-        <f>C50-F50</f>
+        <f t="shared" si="2"/>
         <v>1.99</v>
       </c>
       <c r="E50">
-        <f>C50+F50</f>
+        <f t="shared" si="3"/>
         <v>2.0099999999999998</v>
       </c>
       <c r="F50">
@@ -1778,7 +1778,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -1787,11 +1787,11 @@
         <v>1.2</v>
       </c>
       <c r="D51">
-        <f>C51-F51</f>
+        <f t="shared" si="2"/>
         <v>1.19</v>
       </c>
       <c r="E51">
-        <f>C51+F51</f>
+        <f t="shared" si="3"/>
         <v>1.21</v>
       </c>
       <c r="F51">
@@ -1806,7 +1806,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -1815,11 +1815,11 @@
         <v>0.4</v>
       </c>
       <c r="D52">
-        <f>C52-F52</f>
+        <f t="shared" si="2"/>
         <v>0.39</v>
       </c>
       <c r="E52">
-        <f>C52+F52</f>
+        <f t="shared" si="3"/>
         <v>0.41000000000000003</v>
       </c>
       <c r="F52">
@@ -1834,7 +1834,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
         <v>58</v>
@@ -1849,7 +1849,7 @@
         <v>62.6</v>
       </c>
       <c r="F53">
-        <f>E53-C53</f>
+        <f t="shared" ref="F53:F58" si="4">E53-C53</f>
         <v>0.70000000000000284</v>
       </c>
       <c r="G53">
@@ -1861,7 +1861,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -1876,7 +1876,7 @@
         <v>22.4</v>
       </c>
       <c r="F54">
-        <f>E54-C54</f>
+        <f t="shared" si="4"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="G54">
@@ -1888,7 +1888,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1903,7 +1903,7 @@
         <v>10.5</v>
       </c>
       <c r="F55">
-        <f>E55-C55</f>
+        <f t="shared" si="4"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="G55">
@@ -1915,7 +1915,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
         <v>20</v>
@@ -1930,7 +1930,7 @@
         <v>3</v>
       </c>
       <c r="F56">
-        <f>E56-C56</f>
+        <f t="shared" si="4"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G56">
@@ -1942,7 +1942,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B57" t="s">
         <v>59</v>
@@ -1957,7 +1957,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F57">
-        <f>E57-C57</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G57">
@@ -1969,7 +1969,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
         <v>60</v>
@@ -1984,7 +1984,7 @@
         <v>0.8</v>
       </c>
       <c r="F58">
-        <f>E58-C58</f>
+        <f t="shared" si="4"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G58">
@@ -1996,7 +1996,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
         <v>61</v>
@@ -2028,7 +2028,7 @@
         <v>46.54</v>
       </c>
       <c r="F60">
-        <f>E60-C60</f>
+        <f t="shared" ref="F60:F91" si="5">E60-C60</f>
         <v>0.64999999999999858</v>
       </c>
       <c r="G60">
@@ -2055,7 +2055,7 @@
         <v>28.66</v>
       </c>
       <c r="F61">
-        <f>E61-C61</f>
+        <f t="shared" si="5"/>
         <v>0.67000000000000171</v>
       </c>
       <c r="G61">
@@ -2082,7 +2082,7 @@
         <v>13.27</v>
       </c>
       <c r="F62">
-        <f>E62-C62</f>
+        <f t="shared" si="5"/>
         <v>0.41999999999999993</v>
       </c>
       <c r="G62">
@@ -2109,7 +2109,7 @@
         <v>5.51</v>
       </c>
       <c r="F63">
-        <f>E63-C63</f>
+        <f t="shared" si="5"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="G63">
@@ -2136,7 +2136,7 @@
         <v>2.64</v>
       </c>
       <c r="F64">
-        <f>E64-C64</f>
+        <f t="shared" si="5"/>
         <v>0.12000000000000011</v>
       </c>
       <c r="G64">
@@ -2163,7 +2163,7 @@
         <v>2.38</v>
       </c>
       <c r="F65">
-        <f>E65-C65</f>
+        <f t="shared" si="5"/>
         <v>0.10999999999999988</v>
       </c>
       <c r="G65">
@@ -2190,7 +2190,7 @@
         <v>1.25</v>
       </c>
       <c r="F66">
-        <f>E66-C66</f>
+        <f t="shared" si="5"/>
         <v>8.0000000000000071E-2</v>
       </c>
       <c r="G66">
@@ -2217,7 +2217,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="F67">
-        <f>E67-C67</f>
+        <f t="shared" si="5"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="G67">
@@ -2244,7 +2244,7 @@
         <v>0.44</v>
       </c>
       <c r="F68">
-        <f>E68-C68</f>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="G68">
@@ -2271,7 +2271,7 @@
         <v>0.39</v>
       </c>
       <c r="F69">
-        <f>E69-C69</f>
+        <f t="shared" si="5"/>
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="G69">
@@ -2298,7 +2298,7 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="F70">
-        <f>E70-C70</f>
+        <f t="shared" si="5"/>
         <v>9.0000000000000024E-2</v>
       </c>
       <c r="G70">
@@ -2325,7 +2325,7 @@
         <v>0.39</v>
       </c>
       <c r="F71">
-        <f>E71-C71</f>
+        <f t="shared" si="5"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="G71">
@@ -2352,7 +2352,7 @@
         <v>0.17</v>
       </c>
       <c r="F72">
-        <f>E72-C72</f>
+        <f t="shared" si="5"/>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="G72">
@@ -2379,7 +2379,7 @@
         <v>0.12000000000000001</v>
       </c>
       <c r="F73">
-        <f>E73-C73</f>
+        <f t="shared" si="5"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="G73">
@@ -2406,7 +2406,7 @@
         <v>50</v>
       </c>
       <c r="F74">
-        <f>E74-C74</f>
+        <f t="shared" si="5"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="G74">
@@ -2433,7 +2433,7 @@
         <v>27.700000000000003</v>
       </c>
       <c r="F75">
-        <f>E75-C75</f>
+        <f t="shared" si="5"/>
         <v>0.90000000000000213</v>
       </c>
       <c r="G75">
@@ -2460,7 +2460,7 @@
         <v>5.2</v>
       </c>
       <c r="F76">
-        <f>E76-C76</f>
+        <f t="shared" si="5"/>
         <v>0.29999999999999982</v>
       </c>
       <c r="G76">
@@ -2487,7 +2487,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="F77">
-        <f>E77-C77</f>
+        <f t="shared" si="5"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="G77">
@@ -2514,7 +2514,7 @@
         <v>3.8</v>
       </c>
       <c r="F78">
-        <f>E78-C78</f>
+        <f t="shared" si="5"/>
         <v>0.29999999999999938</v>
       </c>
       <c r="G78">
@@ -2541,7 +2541,7 @@
         <v>3.5999999999999996</v>
       </c>
       <c r="F79">
-        <f>E79-C79</f>
+        <f t="shared" si="5"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="G79">
@@ -2568,7 +2568,7 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="F80">
-        <f>E80-C80</f>
+        <f t="shared" si="5"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G80">
@@ -2595,7 +2595,7 @@
         <v>1.6</v>
       </c>
       <c r="F81">
-        <f>E81-C81</f>
+        <f t="shared" si="5"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G81">
@@ -2622,7 +2622,7 @@
         <v>51.25</v>
       </c>
       <c r="F82">
-        <f>E82-C82</f>
+        <f t="shared" si="5"/>
         <v>0.60999999999999943</v>
       </c>
       <c r="G82">
@@ -2649,7 +2649,7 @@
         <v>18</v>
       </c>
       <c r="F83">
-        <f>E83-C83</f>
+        <f t="shared" si="5"/>
         <v>0.48000000000000043</v>
       </c>
       <c r="G83">
@@ -2676,7 +2676,7 @@
         <v>17.21</v>
       </c>
       <c r="F84">
-        <f>E84-C84</f>
+        <f t="shared" si="5"/>
         <v>0.41000000000000014</v>
       </c>
       <c r="G84">
@@ -2703,7 +2703,7 @@
         <v>7.38</v>
       </c>
       <c r="F85">
-        <f>E85-C85</f>
+        <f t="shared" si="5"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="G85">
@@ -2730,7 +2730,7 @@
         <v>3.17</v>
       </c>
       <c r="F86">
-        <f>E86-C86</f>
+        <f t="shared" si="5"/>
         <v>0.12999999999999989</v>
       </c>
       <c r="G86">
@@ -2757,7 +2757,7 @@
         <v>2.09</v>
       </c>
       <c r="F87">
-        <f>E87-C87</f>
+        <f t="shared" si="5"/>
         <v>0.10999999999999988</v>
       </c>
       <c r="G87">
@@ -2784,7 +2784,7 @@
         <v>1.39</v>
       </c>
       <c r="F88">
-        <f>E88-C88</f>
+        <f t="shared" si="5"/>
         <v>6.999999999999984E-2</v>
       </c>
       <c r="G88">
@@ -2811,7 +2811,7 @@
         <v>1.03</v>
       </c>
       <c r="F89">
-        <f>E89-C89</f>
+        <f t="shared" si="5"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="G89">
@@ -2838,7 +2838,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="F90">
-        <f>E90-C90</f>
+        <f t="shared" si="5"/>
         <v>2.9999999999999971E-2</v>
       </c>
       <c r="G90">
@@ -2865,7 +2865,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F91">
-        <f>E91-C91</f>
+        <f t="shared" si="5"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="G91">
@@ -2892,7 +2892,7 @@
         <v>0.11</v>
       </c>
       <c r="F92">
-        <f>E92-C92</f>
+        <f t="shared" ref="F92:F123" si="6">E92-C92</f>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="G92">
@@ -2919,7 +2919,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F93">
-        <f>E93-C93</f>
+        <f t="shared" si="6"/>
         <v>1.0000000000000009E-2</v>
       </c>
       <c r="G93">
@@ -2946,7 +2946,7 @@
         <v>0.06</v>
       </c>
       <c r="F94">
-        <f>E94-C94</f>
+        <f t="shared" si="6"/>
         <v>9.999999999999995E-3</v>
       </c>
       <c r="G94">
@@ -2958,7 +2958,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B95" t="s">
         <v>4</v>
@@ -2973,7 +2973,7 @@
         <v>38.5</v>
       </c>
       <c r="F95">
-        <f>E95-C95</f>
+        <f t="shared" si="6"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="G95">
@@ -2985,7 +2985,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -3000,7 +3000,7 @@
         <v>39.5</v>
       </c>
       <c r="F96">
-        <f>E96-C96</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G96">
@@ -3012,7 +3012,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -3027,7 +3027,7 @@
         <v>11.5</v>
       </c>
       <c r="F97">
-        <f>E97-C97</f>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="G97">
@@ -3039,7 +3039,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
@@ -3054,7 +3054,7 @@
         <v>4</v>
       </c>
       <c r="F98">
-        <f>E98-C98</f>
+        <f t="shared" si="6"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G98">
@@ -3066,7 +3066,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B99" t="s">
         <v>34</v>
@@ -3081,7 +3081,7 @@
         <v>2.5</v>
       </c>
       <c r="F99">
-        <f>E99-C99</f>
+        <f t="shared" si="6"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G99">
@@ -3093,7 +3093,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B100" t="s">
         <v>35</v>
@@ -3108,7 +3108,7 @@
         <v>2.4</v>
       </c>
       <c r="F100">
-        <f>E100-C100</f>
+        <f t="shared" si="6"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="G100">
@@ -3120,7 +3120,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B101" t="s">
         <v>36</v>
@@ -3135,7 +3135,7 @@
         <v>1.4</v>
       </c>
       <c r="F101">
-        <f>E101-C101</f>
+        <f t="shared" si="6"/>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="G101">
@@ -3147,7 +3147,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B102" t="s">
         <v>4</v>
@@ -3162,7 +3162,7 @@
         <v>59.9</v>
       </c>
       <c r="F102">
-        <f>E102-C102</f>
+        <f t="shared" si="6"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="G102">
@@ -3174,7 +3174,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
@@ -3189,7 +3189,7 @@
         <v>41.7</v>
       </c>
       <c r="F103">
-        <f>E103-C103</f>
+        <f t="shared" si="6"/>
         <v>0.80000000000000426</v>
       </c>
       <c r="G103">
@@ -3216,7 +3216,7 @@
         <v>46.5</v>
       </c>
       <c r="F104">
-        <f>E104-C104</f>
+        <f t="shared" si="6"/>
         <v>0.69999999999999574</v>
       </c>
       <c r="G104">
@@ -3243,7 +3243,7 @@
         <v>27</v>
       </c>
       <c r="F105">
-        <f>E105-C105</f>
+        <f t="shared" si="6"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="G105">
@@ -3270,7 +3270,7 @@
         <v>3.9</v>
       </c>
       <c r="F106">
-        <f>E106-C106</f>
+        <f t="shared" si="6"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G106">
@@ -3297,7 +3297,7 @@
         <v>3.2</v>
       </c>
       <c r="F107">
-        <f>E107-C107</f>
+        <f t="shared" si="6"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G107">
@@ -3324,7 +3324,7 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="F108">
-        <f>E108-C108</f>
+        <f t="shared" si="6"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="G108">
@@ -3351,7 +3351,7 @@
         <v>3.1</v>
       </c>
       <c r="F109">
-        <f>E109-C109</f>
+        <f t="shared" si="6"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G109">
@@ -3378,7 +3378,7 @@
         <v>3</v>
       </c>
       <c r="F110">
-        <f>E110-C110</f>
+        <f t="shared" si="6"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="G110">
@@ -3405,7 +3405,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="F111">
-        <f>E111-C111</f>
+        <f t="shared" si="6"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G111">
@@ -3432,7 +3432,7 @@
         <v>1.0999999999999999</v>
       </c>
       <c r="F112">
-        <f>E112-C112</f>
+        <f t="shared" si="6"/>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="G112">
@@ -3459,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="F113">
-        <f>E113-C113</f>
+        <f t="shared" si="6"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="G113">

</xml_diff>